<commit_message>
Coding Ninja - Count Number of Distinct Substring in array
Coding Ninja - Count Number of Distinct Substring in array and documentation updated
</commit_message>
<xml_diff>
--- a/Trie/Question_List-Java version.xlsx
+++ b/Trie/Question_List-Java version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Trie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FF8266-CACA-41A6-BBBD-9A158BE78D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9CA209-A539-4EB6-A590-47E35D3A03ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Question No</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Implement Trie (Prefix Tree)</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Longest Word With All Prefixes</t>
+  </si>
+  <si>
+    <t>Count Distinct Substrings</t>
   </si>
 </sst>
 </file>
@@ -143,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -180,29 +189,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +478,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,187 +516,202 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="5">
         <v>208</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:7" s="15" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="18"/>
-    </row>
-    <row r="4" spans="1:7" s="15" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="1:7" s="15" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:7" s="15" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" s="15" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:7" s="15" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" s="15" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:7" s="15" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="15" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="14"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D25" s="7"/>

</xml_diff>